<commit_message>
aggiunta test_case ID:28 al file report_checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-LAB/3.15.0.0/report_checklist.xlsx
+++ b/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-LAB/3.15.0.0/report_checklist.xlsx
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.6cbb54898ba2300f36707c2acfc06610f72746722d8001b4fc688e0796a3fdd5.f193d4184b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t xml:space="preserve">NOME FORNITORE:</t>
   </si>
@@ -222,6 +219,60 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.bed50d45f5cc52a65ca0bd4d8f32ee276de7fa32243db0ad21c6aede1b7bfff7.8cfdf34d5e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
+    <t>VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u val="single"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u val="single"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario non valorizzare nel JWT il campo "purpose_of_use".</t>
+    </r>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il token viene sempre e comunque compilato dal software che non ammette campi vuoti in questa fase.</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO</t>
   </si>
   <si>
@@ -267,9 +318,6 @@
     </r>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>2023-07-25T12:31:00Z</t>
   </si>
   <si>
@@ -285,9 +333,6 @@
     <t xml:space="preserve">Nel software viene visualizzato l'errore “Campo JWT non valido:"piu la descrizione esatta dell'errore ricevuto. Il referto vine memorizzato in un apposita lista di lavoro dal quale è possibile effettuare le opportune correzioni per poi procedere con un nuovo invio del documento alla validazione.</t>
   </si>
   <si>
-    <t>KO</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
   </si>
   <si>
@@ -296,9 +341,6 @@
   </si>
   <si>
     <t xml:space="preserve">TimeOut error: non è stato possibile inviare in validazione il seguente referto: "nr referto"</t>
-  </si>
-  <si>
-    <t>NO</t>
   </si>
   <si>
     <t xml:space="preserve">Nel caso di TimeOut viene segnalato all'utente tramite messaggio a video l'impossibilità di invio e il referto prodotto vine memorizzato in un apposita lista dal quale sarà possibile effettuare un nuovo invio  alla validazione</t>
@@ -343,7 +385,7 @@
     <t xml:space="preserve">[ERRORE-6| L'elemento  'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code  valorizzato con 'N' o 'V', e il suo @codeSystem  con '2.16.840.1.113883.5.25']</t>
   </si>
   <si>
-    <t xml:space="preserve">Il confidentialityCode viene selezionato dall'apposita combobox nella maschera di inserimento valorizzata secondo normativa, quall'ora questa presentasse dei valori non corretti derivati da una configurazzione errata è possibile richiederne la correzione al backoffice.
+    <t xml:space="preserve">Il confidentialityCode viene selezionato dall'apposita combobox nella maschera di inserimento valorizzata secondo normativa, qualora questa presentasse dei valori non corretti derivati da una configurazzione errata è possibile richiederne la correzione al backoffice.
 Il documento CDA viene scartato ed è possibile rigenerarlo una volta effettuate le opportune correzioni.</t>
   </si>
   <si>
@@ -413,7 +455,7 @@
     <t xml:space="preserve">[ERRORE-b1| L'elemento code della section DEVE essere valorizzato con uno dei seguenti codici LOINC individuati:\n\t\t\t\t\t\t18717-9 BANCA DEL SANGUE\n\t\t\t\t\t\t18718-7 MARCATORI CELLULARI \n\t\t\t\t\t\t18719-5 CHIMICA\n\t\t\t\t\t\t18720-3\tCOAGULAZIONE\n\t\t\t\t\t\t18721-1 MONITORAGGIO TERAPEUTICO DEI FARMACI\n\t\t\t\t\t\t18722-9 FERTILITÃ€\n\t\t\t\t\t\t18723-7 EMATOLOGIA\n\t\t\t\t\t\t18724-5 HLA\n\t\t\t\t\t\t18725-2 MICROBIOLOGIA\n\t\t\t\t\t\t18727-8 SEROLOGIA\n\t\t\t\t\t\t18728-6 TOSSICOLOGIA\n\t\t\t\t\t\t18729-4 ESAMI DELLE URINE\n\t\t\t\t\t\t18767-4 EMOGASANALISI\n\t\t\t\t\t\t18768-2 CONTE CELLULARE+DIFFERENZIALE\n\t\t\t\t\t\t18769-0 SUSCETTIBILITÃ€ ANTIMICROBICA\n\t\t\t\t\t\t26435-8 PATOLOGIA MOLECOLARE\n\t\t\t\t\t\t26436-6 ESAMI DI LABORATORIO\n\t\t\t\t\t\t26437-4 TEST DI SENSIBILITÃ€ A SOSTANZE CHIMICHE\n\t\t\t\t\t\t26438-2 CITOLOGIA\n\t\t\t\t\t\t18716-1 ALLERGOLOGIA\n\t\t\t\t\t\t26439-0 PATOLOGIA CHIRURGICA],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ]</t>
   </si>
   <si>
-    <t xml:space="preserve">Il section/code contentente la "specialità di laboratorio" viene selezionato dall'apposita combobox nella maschera di valorizazione esame, quall'ora questa presentasse dei valori non corretti derivati da una configurazzione errata è possibile richiederne la correzione al backoffice.
+    <t xml:space="preserve">Il section/code contentente la "specialità di laboratorio" viene selezionato dall'apposita combobox nella maschera di valorizazione esame, qualora questa presentasse dei valori non corretti derivati da una configurazzione errata è possibile richiederne la correzione al backoffice.
 Il documento CDA viene scartato ed è possibile rigenerarlo una volta effettuate le opportune correzioni.</t>
   </si>
   <si>
@@ -450,6 +492,9 @@
   </si>
   <si>
     <t>099fc9ea0a39b987</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.6cbb54898ba2300f36707c2acfc06610f72746722d8001b4fc688e0796a3fdd5.f193d4184b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Errore di sintassi.","detail":"ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'code' is not valid with respect to its type, 'cs'.,ERROR: -1,-1 cvc-minLength-valid: Value '' with length = '0' is not facet-valid with respect to minLength '1' for type 'st'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'displayName' on element 'code' is not valid with respect to its type, 'st'</t>
@@ -529,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="24">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -723,12 +768,103 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="none"/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="50">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -833,6 +969,48 @@
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="18" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="18" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="18" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="22" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="22" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="6" fillId="4" borderId="14" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1346,7 +1524,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G27" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1376,9 +1554,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="409.5">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
@@ -1401,11 +1577,11 @@
     </row>
     <row r="2" ht="18.75">
       <c r="A2" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="4"/>
@@ -1427,11 +1603,11 @@
     </row>
     <row r="3" ht="16.5">
       <c r="A3" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="4"/>
@@ -1455,7 +1631,7 @@
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="7"/>
@@ -1479,7 +1655,7 @@
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="4"/>
@@ -1567,64 +1743,64 @@
     </row>
     <row r="9" ht="18.75">
       <c r="A9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="D9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="E9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="F9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="G9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="H9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="I9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="J9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="K9" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="L9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="M9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="26" t="s">
+      <c r="N9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="26" t="s">
+      <c r="O9" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="O9" s="26" t="s">
+      <c r="P9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="26" t="s">
+      <c r="Q9" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="26" t="s">
+      <c r="R9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="27" t="s">
+      <c r="S9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="S9" s="26" t="s">
+      <c r="T9" s="26" t="s">
         <v>25</v>
-      </c>
-      <c r="T9" s="26" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" ht="156.75">
@@ -1632,31 +1808,31 @@
         <v>1</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="D10" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="E10" s="30" t="s">
         <v>29</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>30</v>
       </c>
       <c r="F10" s="31">
         <v>45132</v>
       </c>
       <c r="G10" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="I10" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="J10" s="29" t="s">
         <v>33</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>34</v>
       </c>
       <c r="K10" s="29"/>
       <c r="L10" s="29"/>
@@ -1668,7 +1844,7 @@
       <c r="R10" s="32"/>
       <c r="S10" s="33"/>
       <c r="T10" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" ht="156.75">
@@ -1676,31 +1852,31 @@
         <v>2</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>37</v>
       </c>
       <c r="F11" s="31">
         <v>45132</v>
       </c>
       <c r="G11" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="I11" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="31" t="s">
-        <v>40</v>
-      </c>
       <c r="J11" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
@@ -1712,7 +1888,7 @@
       <c r="R11" s="32"/>
       <c r="S11" s="33"/>
       <c r="T11" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" ht="156.75">
@@ -1720,31 +1896,31 @@
         <v>3</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D12" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>42</v>
       </c>
       <c r="F12" s="31">
         <v>45132</v>
       </c>
       <c r="G12" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="I12" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="31" t="s">
-        <v>45</v>
-      </c>
       <c r="J12" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K12" s="29"/>
       <c r="L12" s="29"/>
@@ -1756,7 +1932,7 @@
       <c r="R12" s="32"/>
       <c r="S12" s="33"/>
       <c r="T12" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" ht="156.75">
@@ -1764,31 +1940,31 @@
         <v>4</v>
       </c>
       <c r="B13" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>46</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>47</v>
       </c>
       <c r="F13" s="31">
         <v>45132</v>
       </c>
       <c r="G13" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="I13" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="31" t="s">
-        <v>50</v>
-      </c>
       <c r="J13" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="29"/>
       <c r="L13" s="29"/>
@@ -1800,7 +1976,7 @@
       <c r="R13" s="32"/>
       <c r="S13" s="33"/>
       <c r="T13" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" ht="156.75">
@@ -1808,31 +1984,31 @@
         <v>5</v>
       </c>
       <c r="B14" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D14" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>52</v>
       </c>
       <c r="F14" s="31">
         <v>45132</v>
       </c>
       <c r="G14" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="I14" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="31" t="s">
-        <v>55</v>
-      </c>
       <c r="J14" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
@@ -1844,174 +2020,174 @@
       <c r="R14" s="32"/>
       <c r="S14" s="33"/>
       <c r="T14" s="34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" ht="228">
-      <c r="A15" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" ht="156.75">
+      <c r="A15" s="35">
+        <v>28</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" ht="228">
+      <c r="A16" s="42">
         <v>36</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B16" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="31" t="s">
+      <c r="D16" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="45">
+        <v>45132</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="N15" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="O15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="P15" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="33"/>
-      <c r="T15" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" ht="156.75">
-      <c r="A16" s="28">
+    </row>
+    <row r="17" ht="156.75">
+      <c r="A17" s="28">
         <v>44</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B17" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="N16" s="29" t="s">
+      <c r="D17" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="E17" s="30" t="s">
         <v>68</v>
-      </c>
-      <c r="P16" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="S16" s="33"/>
-      <c r="T16" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" ht="114">
-      <c r="A17" s="28">
-        <v>52</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>71</v>
       </c>
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
       <c r="J17" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="K17" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
+        <v>33</v>
+      </c>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>70</v>
+      </c>
       <c r="Q17" s="29"/>
-      <c r="R17" s="32"/>
+      <c r="R17" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="S17" s="33"/>
       <c r="T17" s="34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" ht="114">
       <c r="A18" s="28">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D18" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
       <c r="J18" s="29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="K18" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
@@ -2022,124 +2198,124 @@
       <c r="R18" s="32"/>
       <c r="S18" s="33"/>
       <c r="T18" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" ht="256.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" ht="114">
       <c r="A19" s="28">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="31">
-        <v>45132</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="29" t="s">
-        <v>81</v>
-      </c>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
       <c r="O19" s="29"/>
-      <c r="P19" s="29" t="s">
-        <v>82</v>
-      </c>
+      <c r="P19" s="29"/>
       <c r="Q19" s="29"/>
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
       <c r="T19" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" ht="114">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" ht="256.5">
       <c r="A20" s="28">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D20" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="31">
+        <v>45132</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="K20" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="29"/>
       <c r="Q20" s="29"/>
       <c r="R20" s="32"/>
       <c r="S20" s="33"/>
       <c r="T20" s="34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" ht="114">
       <c r="A21" s="28">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D21" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
       <c r="J21" s="29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="K21" s="29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
@@ -2150,34 +2326,34 @@
       <c r="R21" s="32"/>
       <c r="S21" s="33"/>
       <c r="T21" s="34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" ht="114">
       <c r="A22" s="28">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D22" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="30" t="s">
         <v>88</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>89</v>
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
       <c r="J22" s="29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="K22" s="29" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
@@ -2188,34 +2364,34 @@
       <c r="R22" s="32"/>
       <c r="S22" s="33"/>
       <c r="T22" s="34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" ht="114">
       <c r="A23" s="28">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D23" s="29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
       <c r="J23" s="29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="K23" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L23" s="29"/>
       <c r="M23" s="29"/>
@@ -2226,34 +2402,34 @@
       <c r="R23" s="32"/>
       <c r="S23" s="33"/>
       <c r="T23" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" ht="128.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" ht="114">
       <c r="A24" s="28">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D24" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="K24" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
@@ -2264,190 +2440,206 @@
       <c r="R24" s="32"/>
       <c r="S24" s="33"/>
       <c r="T24" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" ht="409.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" ht="128.25">
       <c r="A25" s="28">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D25" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="K25" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="31">
-        <v>45132</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="I25" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="O25" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="P25" s="29" t="s">
-        <v>103</v>
-      </c>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
       <c r="R25" s="32"/>
       <c r="S25" s="33"/>
       <c r="T25" s="34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" ht="409.5">
       <c r="A26" s="28">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D26" s="29" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F26" s="31">
         <v>45132</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I26" s="31" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K26" s="29"/>
       <c r="L26" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M26" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="N26" s="29" t="s">
-        <v>109</v>
+        <v>33</v>
+      </c>
+      <c r="N26" s="49" t="s">
+        <v>103</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P26" s="29" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="Q26" s="29"/>
       <c r="R26" s="32"/>
       <c r="S26" s="33"/>
       <c r="T26" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" ht="270.75">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" ht="409.5">
       <c r="A27" s="28">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>28</v>
-      </c>
       <c r="D27" s="29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F27" s="31">
         <v>45132</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I27" s="31" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K27" s="29"/>
       <c r="L27" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M27" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="O27" s="29"/>
+        <v>33</v>
+      </c>
+      <c r="N27" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="O27" s="29" t="s">
+        <v>33</v>
+      </c>
       <c r="P27" s="29" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="Q27" s="29"/>
       <c r="R27" s="32"/>
       <c r="S27" s="33"/>
       <c r="T27" s="34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="5"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" ht="270.75">
+      <c r="A28" s="28">
+        <v>62</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="31">
+        <v>45132</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="33"/>
+      <c r="T28" s="34" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="4"/>
@@ -6833,20 +7025,20 @@
       <c r="C228" s="4"/>
       <c r="D228" s="4"/>
       <c r="E228" s="4"/>
-      <c r="F228" s="4"/>
-      <c r="G228" s="4"/>
-      <c r="H228" s="4"/>
-      <c r="I228" s="4"/>
-      <c r="J228" s="4"/>
-      <c r="K228" s="4"/>
-      <c r="L228" s="4"/>
-      <c r="M228" s="4"/>
-      <c r="N228" s="4"/>
-      <c r="O228" s="4"/>
-      <c r="P228" s="4"/>
-      <c r="Q228" s="4"/>
-      <c r="R228" s="4"/>
-      <c r="S228" s="4"/>
+      <c r="F228" s="5"/>
+      <c r="G228" s="5"/>
+      <c r="H228" s="5"/>
+      <c r="I228" s="5"/>
+      <c r="J228" s="5"/>
+      <c r="K228" s="5"/>
+      <c r="L228" s="5"/>
+      <c r="M228" s="5"/>
+      <c r="N228" s="5"/>
+      <c r="O228" s="5"/>
+      <c r="P228" s="5"/>
+      <c r="Q228" s="5"/>
+      <c r="R228" s="6"/>
+      <c r="S228" s="7"/>
       <c r="T228" s="5"/>
     </row>
     <row r="229" ht="14.25">
@@ -16002,26 +16194,26 @@
       <c r="T644" s="5"/>
     </row>
     <row r="645" ht="14.25">
-      <c r="A645" s="1"/>
-      <c r="B645" s="1"/>
-      <c r="C645" s="1"/>
-      <c r="D645" s="1"/>
-      <c r="E645" s="1"/>
-      <c r="F645" s="1"/>
-      <c r="G645" s="1"/>
-      <c r="H645" s="1"/>
-      <c r="I645" s="1"/>
-      <c r="J645" s="1"/>
-      <c r="K645" s="1"/>
-      <c r="L645" s="1"/>
-      <c r="M645" s="1"/>
-      <c r="N645" s="1"/>
-      <c r="O645" s="1"/>
-      <c r="P645" s="1"/>
-      <c r="Q645" s="1"/>
-      <c r="R645" s="1"/>
-      <c r="S645" s="1"/>
-      <c r="T645" s="1"/>
+      <c r="A645" s="4"/>
+      <c r="B645" s="4"/>
+      <c r="C645" s="4"/>
+      <c r="D645" s="4"/>
+      <c r="E645" s="4"/>
+      <c r="F645" s="4"/>
+      <c r="G645" s="4"/>
+      <c r="H645" s="4"/>
+      <c r="I645" s="4"/>
+      <c r="J645" s="4"/>
+      <c r="K645" s="4"/>
+      <c r="L645" s="4"/>
+      <c r="M645" s="4"/>
+      <c r="N645" s="4"/>
+      <c r="O645" s="4"/>
+      <c r="P645" s="4"/>
+      <c r="Q645" s="4"/>
+      <c r="R645" s="4"/>
+      <c r="S645" s="4"/>
+      <c r="T645" s="5"/>
     </row>
     <row r="646" ht="14.25">
       <c r="A646" s="1"/>
@@ -16045,6 +16237,28 @@
       <c r="S646" s="1"/>
       <c r="T646" s="1"/>
     </row>
+    <row r="647" ht="14.25">
+      <c r="A647" s="1"/>
+      <c r="B647" s="1"/>
+      <c r="C647" s="1"/>
+      <c r="D647" s="1"/>
+      <c r="E647" s="1"/>
+      <c r="F647" s="1"/>
+      <c r="G647" s="1"/>
+      <c r="H647" s="1"/>
+      <c r="I647" s="1"/>
+      <c r="J647" s="1"/>
+      <c r="K647" s="1"/>
+      <c r="L647" s="1"/>
+      <c r="M647" s="1"/>
+      <c r="N647" s="1"/>
+      <c r="O647" s="1"/>
+      <c r="P647" s="1"/>
+      <c r="Q647" s="1"/>
+      <c r="R647" s="1"/>
+      <c r="S647" s="1"/>
+      <c r="T647" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A2:B2"/>
@@ -16055,11 +16269,17 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <dataValidations count="2" disablePrompts="0">
-    <dataValidation sqref="J28:J32 L10:M14 L17:M18 L20:M24 L28:M32 O10:O14 O17:O24 O27 O28:O32 J34 L34:M34 O34 J36:J40 L36:M40 O36:O40 J42 L42:M42 O42 J44:J48 L44:M48 O44:O48 J50:J194 L50:M194 O50:O194 J371:J379 L371:M379 O371:O379" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+  <dataValidations count="4" disablePrompts="0">
+    <dataValidation sqref="J29:J33 L10:M14 L18:M19 L21:M25 L29:M33 O10:O14 O18:O25 O28 O29:O33 J35 L35:M35 O35 J37:J41 L37:M41 O37:O41 J43 L43:M43 O43 J45:J49 L45:M49 O45:O49 J51:J195 L51:M195 O51:O195 J372:J380 L372:M380 O372:O380" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$B$2:$B$3</formula1>
     </dataValidation>
-    <dataValidation sqref="Q10:Q27 Q28:Q32 Q34 Q36:Q40 Q42 Q44:Q48 Q50:Q194 Q371:Q379" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="Q10:Q14 Q16:Q28 Q29:Q33 Q35 Q37:Q41 Q43 Q45:Q49 Q51:Q195 Q372:Q380" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$A$2:$A$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="L15:M15 O15" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>Sheet1!$B$2:$B$3</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q15" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>Sheet1!$A$2:$A$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adeguamento post segnalazioni del 31/07/2023
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-LAB/3.15.0.0/report_checklist.xlsx
+++ b/GATEWAY/A1#111DMEDICALSRLXX/D-MEDICAL_SRL/MEDINET-LAB/3.15.0.0/report_checklist.xlsx
@@ -132,13 +132,13 @@
 </t>
   </si>
   <si>
-    <t>2023-07-25T10:26:00Z</t>
+    <t>2023-08-10T14:11:53Z</t>
   </si>
   <si>
-    <t>4fceabfbaf25eba7</t>
+    <t>123ca635cfc7125b</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.e9697770c97c8a86cf58c28a5c4f7437054bfbf756a170d118f4541079118d9f.3cd70c09b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.e9697770c97c8a86cf58c28a5c4f7437054bfbf756a170d118f4541079118d9f.5a5acd1d07^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -156,13 +156,13 @@
 </t>
   </si>
   <si>
-    <t>2023-07-25T10:36:00Z</t>
+    <t>2023-08-10T14:26:53Z</t>
   </si>
   <si>
-    <t>aff136d6ad363048</t>
+    <t>7ea6c956c369e7b5</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.3aa62f1983c890325821d77d140469655c23b28cbdb1760936c7c58c44a65548.2282849e52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.3aa62f1983c890325821d77d140469655c23b28cbdb1760936c7c58c44a65548.851e7e93e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT3</t>
@@ -174,13 +174,13 @@
 </t>
   </si>
   <si>
-    <t>2023-07-25T11:55:00Z</t>
+    <t>2023-08-10T14:29:06Z</t>
   </si>
   <si>
-    <t>80c0c379282219a0</t>
+    <t>ce61ec82b3d7cb57</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.682bef12c7c5498ec50f074cd063e98b13d1d6e4a095eb7dd439cbbf881019e4.4c3945f797^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.682bef12c7c5498ec50f074cd063e98b13d1d6e4a095eb7dd439cbbf881019e4.f612345623^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT4</t>
@@ -192,13 +192,13 @@
 </t>
   </si>
   <si>
-    <t>2023-07-25T11:57:00Z</t>
+    <t>2023-08-10T14:30:14Z</t>
   </si>
   <si>
-    <t>8071e9127e9f7fd6</t>
+    <t>bdeff6457c3462c6</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.ab2a288383d0733a53b63afdec35af9e22a0511baeb0b803457b5fc733aee2cb.5ddb3fa4bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.ab2a288383d0733a53b63afdec35af9e22a0511baeb0b803457b5fc733aee2cb.9675216d8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LAB_CT5</t>
@@ -210,13 +210,13 @@
 </t>
   </si>
   <si>
-    <t>2023-07-25T12:07:00Z</t>
+    <t>2023-08-10T14:31:35Z</t>
   </si>
   <si>
-    <t>5c4064eaf3091d2d</t>
+    <t>ed218f78fee2ce6c</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.bed50d45f5cc52a65ca0bd4d8f32ee276de7fa32243db0ad21c6aede1b7bfff7.8cfdf34d5e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.bed50d45f5cc52a65ca0bd4d8f32ee276de7fa32243db0ad21c6aede1b7bfff7.19e3808068^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_LAB_KO</t>
@@ -1524,7 +1524,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G12" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1820,7 +1820,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="31">
-        <v>45132</v>
+        <v>45148</v>
       </c>
       <c r="G10" s="31" t="s">
         <v>30</v>
@@ -1864,7 +1864,7 @@
         <v>36</v>
       </c>
       <c r="F11" s="31">
-        <v>45132</v>
+        <v>45148</v>
       </c>
       <c r="G11" s="31" t="s">
         <v>37</v>
@@ -1908,7 +1908,7 @@
         <v>41</v>
       </c>
       <c r="F12" s="31">
-        <v>45132</v>
+        <v>45148</v>
       </c>
       <c r="G12" s="31" t="s">
         <v>42</v>
@@ -1952,7 +1952,7 @@
         <v>46</v>
       </c>
       <c r="F13" s="31">
-        <v>45132</v>
+        <v>45148</v>
       </c>
       <c r="G13" s="31" t="s">
         <v>47</v>
@@ -1996,7 +1996,7 @@
         <v>51</v>
       </c>
       <c r="F14" s="31">
-        <v>45132</v>
+        <v>45148</v>
       </c>
       <c r="G14" s="31" t="s">
         <v>52</v>

</xml_diff>